<commit_message>
FUNCTIONALITY: JobHistory/Read - Wrote the suite. CRUD/Read - Fixed a keyword name.
</commit_message>
<xml_diff>
--- a/QA/Tests/JobHistory/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/JobHistory/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Title</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Testing</t>
+  </si>
+  <si>
+    <t>Read</t>
   </si>
 </sst>
 </file>
@@ -535,7 +538,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +568,7 @@
       </c>
       <c r="E1" s="4">
         <f>COUNTA($A:$A) -1</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
@@ -604,7 +607,18 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D3" s="5"/>
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>7</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="F3" s="3"/>
       <c r="G3" s="7"/>
     </row>
@@ -614,7 +628,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -632,7 +646,7 @@
       </c>
       <c r="G6" s="9">
         <f>G5/G4</f>
-        <v>0.25</v>
+        <v>0.13333333333333333</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
FUNCTIONALITY: Added some suites Updated stats Change a delete keyword to API delete for AppendOverlay
</commit_message>
<xml_diff>
--- a/QA/Tests/JobHistory/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/JobHistory/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Title</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t>Contains a partially automated test case.</t>
+  </si>
+  <si>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -153,7 +162,19 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -541,7 +562,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +592,7 @@
       </c>
       <c r="E1" s="4">
         <f>COUNTA($A:$A) -1</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
@@ -590,16 +611,16 @@
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
         <v>2</v>
       </c>
-      <c r="C2" s="1">
-        <v>8</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>11</v>
+      <c r="D2" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
@@ -611,39 +632,63 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>7</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>7</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G5" s="3">
         <f>SUM($B:$B)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -652,7 +697,7 @@
       </c>
       <c r="G6" s="9">
         <f>G5/G4</f>
-        <v>0.13333333333333333</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -670,35 +715,35 @@
   <sortState ref="A2:E8">
     <sortCondition ref="A2"/>
   </sortState>
-  <conditionalFormatting sqref="D1 D4:D1048576">
-    <cfRule type="containsText" dxfId="8" priority="14" operator="containsText" text="Outdated">
+  <conditionalFormatting sqref="D8:D1048576 D1:D3">
+    <cfRule type="containsText" dxfId="9" priority="14" operator="containsText" text="Outdated">
       <formula>NOT(ISERROR(SEARCH("Outdated",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D3">
-    <cfRule type="containsText" dxfId="7" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
-      <formula>NOT(ISERROR(SEARCH("Finished",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
-      <formula>NOT(ISERROR(SEARCH("Automated",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
-      <formula>NOT(ISERROR(SEARCH("Under Review",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
-      <formula>NOT(ISERROR(SEARCH("Testing",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
-      <formula>NOT(ISERROR(SEARCH("Writing",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
-      <formula>NOT(ISERROR(SEARCH("Ready to Write",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
-      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="8" stopIfTrue="1" operator="containsText" text="Suited to Manual">
-      <formula>NOT(ISERROR(SEARCH("Suited to Manual",D2)))</formula>
+  <conditionalFormatting sqref="D4:D5">
+    <cfRule type="containsText" dxfId="8" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+      <formula>NOT(ISERROR(SEARCH("Finished",D4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+      <formula>NOT(ISERROR(SEARCH("Automated",D4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+      <formula>NOT(ISERROR(SEARCH("Under Review",D4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",D4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+      <formula>NOT(ISERROR(SEARCH("Writing",D4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+      <formula>NOT(ISERROR(SEARCH("Ready to Write",D4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="8" stopIfTrue="1" operator="containsText" text="Suited to Manual">
+      <formula>NOT(ISERROR(SEARCH("Suited to Manual",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FUNCTIONALITY: Delete - Tagged a test case and improved the position for automation. ListView - Finished automating the test suite for now. Read - Added the missing resource file.
</commit_message>
<xml_diff>
--- a/QA/Tests/JobHistory/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/JobHistory/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Title</t>
   </si>
@@ -51,15 +51,9 @@
     <t>ListView</t>
   </si>
   <si>
-    <t>Testing</t>
-  </si>
-  <si>
     <t>Read</t>
   </si>
   <si>
-    <t>Contains a partially automated test case.</t>
-  </si>
-  <si>
     <t>Create</t>
   </si>
   <si>
@@ -70,6 +64,18 @@
   </si>
   <si>
     <t>Writing</t>
+  </si>
+  <si>
+    <t>Contains two partially automated test cases.</t>
+  </si>
+  <si>
+    <t>Contains four partially automated test cases.</t>
+  </si>
+  <si>
+    <t>Ready to Write</t>
+  </si>
+  <si>
+    <t>1 is Automateable, 2/3 are Automateable?</t>
   </si>
 </sst>
 </file>
@@ -165,287 +171,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="41">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF00B0F0"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="180">
-          <stop position="0">
-            <color rgb="FF66FF66"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FF66FF66"/>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF00B0F0"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="180">
-          <stop position="0">
-            <color rgb="FF66FF66"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FF66FF66"/>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF00B0F0"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="180">
-          <stop position="0">
-            <color rgb="FF66FF66"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FF66FF66"/>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF00B0F0"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="180">
-          <stop position="0">
-            <color rgb="FF66FF66"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FF66FF66"/>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF00B0F0"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -821,7 +547,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,40 +584,40 @@
       </c>
       <c r="G1" s="7">
         <f>COUNTIF($D:$D,"Ready to Write")+COUNTIF($D:$D,"Outdated")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="3">
         <f>SUM(G1:G2)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
         <v>2</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="7">
         <f>COUNTIF($D:$D,"Automated")+COUNTIF($D:$D,"Finished")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -900,7 +626,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="7"/>
@@ -910,13 +639,16 @@
         <v>10</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1">
         <v>8</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>7</v>
@@ -928,7 +660,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1">
         <v>8</v>
@@ -937,17 +669,17 @@
         <v>8</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G5" s="3">
         <f>SUM($B:$B)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -956,7 +688,7 @@
       </c>
       <c r="G6" s="9">
         <f>G5/G4</f>
-        <v>0.52380952380952384</v>
+        <v>0.7142857142857143</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -975,30 +707,30 @@
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="15" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="7" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="6" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="5" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="4" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="3" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="2" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="1" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D50">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="23" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="23" stopIfTrue="1">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
FUNCTIONALITY: Completed JobHistoryErrors Automateable Tags in Delete
</commit_message>
<xml_diff>
--- a/QA/Tests/JobHistory/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/JobHistory/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Title</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Ready to Write</t>
+  </si>
+  <si>
+    <t>JobHistoryErrors</t>
   </si>
 </sst>
 </file>
@@ -165,11 +168,78 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="24">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FF66FF66"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
         </patternFill>
       </fill>
     </dxf>
@@ -608,7 +678,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,7 +708,7 @@
       </c>
       <c r="E1" s="4">
         <f>COUNTA($A:$A) -1</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
@@ -652,7 +722,7 @@
       </c>
       <c r="I1" s="3">
         <f>SUM(G1:G2)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -673,7 +743,7 @@
       </c>
       <c r="G2" s="7">
         <f>COUNTIF($D:$D,"Automated")+COUNTIF($D:$D,"Finished")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -694,59 +764,71 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G5" s="3">
         <f>SUM($B:$B)</f>
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="F6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="9">
         <f>G5/G4</f>
-        <v>0.68181818181818177</v>
+        <v>0.70833333333333337</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -764,32 +846,60 @@
   <sortState ref="A2:E8">
     <sortCondition ref="A2"/>
   </sortState>
-  <conditionalFormatting sqref="D1:D1048576">
+  <conditionalFormatting sqref="D1:D3 D5:D1048576">
+    <cfRule type="containsText" dxfId="23" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
+      <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
+      <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
+      <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
+      <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
+      <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D3 D5:D50">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="31" stopIfTrue="1">
+      <formula>LEN(TRIM(D2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
     <cfRule type="containsText" dxfId="15" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
-      <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Finished",D4)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="14" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
-      <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Automated",D4)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="13" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
-      <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Under Review",D4)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="12" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
-      <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Testing",D4)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="11" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
-      <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Writing",D4)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="10" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
-      <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Ready to Write",D4)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="9" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
-      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D50">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="23" stopIfTrue="1">
-      <formula>LEN(TRIM(D2))&gt;0</formula>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="8" stopIfTrue="1">
+      <formula>LEN(TRIM(D4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FUNCTIONALITY: Completed manual tests of JobStats
</commit_message>
<xml_diff>
--- a/QA/Tests/JobHistory/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/JobHistory/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Title</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>JobHistoryErrors</t>
+  </si>
+  <si>
+    <t>JobStatistics</t>
+  </si>
+  <si>
+    <t>JobStatus</t>
+  </si>
+  <si>
+    <t>Suited to Manual</t>
   </si>
 </sst>
 </file>
@@ -168,7 +177,141 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="32">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FF66FF66"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FF66FF66"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -611,7 +754,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,21 +784,21 @@
       </c>
       <c r="E1" s="4">
         <f>COUNTA($A:$A) -1</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="7">
         <f>COUNTIF($D:$D,"Ready to Write")+COUNTIF($D:$D,"Outdated")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="3">
         <f>SUM(G1:G2)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -713,24 +856,21 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
         <v>7</v>
       </c>
-      <c r="C5" s="1">
-        <v>10</v>
-      </c>
       <c r="D5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>8</v>
@@ -742,26 +882,57 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C6" s="1">
-        <v>8</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>16</v>
+        <v>5</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="9">
         <f>G5/G4</f>
-        <v>0.64</v>
+        <v>0.43243243243243246</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1">
+        <v>10</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>8</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -779,60 +950,88 @@
   <sortState ref="A2:E8">
     <sortCondition ref="A2"/>
   </sortState>
-  <conditionalFormatting sqref="D1:D3 D5:D1048576">
-    <cfRule type="containsText" dxfId="15" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
+  <conditionalFormatting sqref="D1:D3 D7:D1048576">
+    <cfRule type="containsText" dxfId="23" priority="17" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="22" priority="18" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="21" priority="19" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="20" priority="20" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="19" priority="21" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="18" priority="22" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="17" priority="23" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D3 D5:D50">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="31" stopIfTrue="1">
+  <conditionalFormatting sqref="D2:D3 D7:D50">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="39" stopIfTrue="1">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="7" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="15" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="14" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="13" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="12" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="11" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="10" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="9" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="16" stopIfTrue="1">
+      <formula>LEN(TRIM(D4))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="containsText" dxfId="7" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+      <formula>NOT(ISERROR(SEARCH("Finished",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+      <formula>NOT(ISERROR(SEARCH("Automated",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+      <formula>NOT(ISERROR(SEARCH("Under Review",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+      <formula>NOT(ISERROR(SEARCH("Writing",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+      <formula>NOT(ISERROR(SEARCH("Ready to Write",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
     <cfRule type="notContainsBlanks" dxfId="0" priority="8" stopIfTrue="1">
-      <formula>LEN(TRIM(D4))&gt;0</formula>
+      <formula>LEN(TRIM(D5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>